<commit_message>
Added Deliverables and changes some
Chase
</commit_message>
<xml_diff>
--- a/Deliverables/4. ProjectSchedule/Schedule-Team4.xlsx
+++ b/Deliverables/4. ProjectSchedule/Schedule-Team4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School Account\Desktop\Team4Project\Deliverables\4. ProjectSchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CFB9F4-597C-4807-BABA-4A4E0863124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8DB26B-D8FE-482E-A2C8-BB913EC23F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="372">
   <si>
     <t>Task#</t>
   </si>
@@ -935,27 +935,6 @@
     <t>Implement Feature 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Clean Up Doc </t>
-  </si>
-  <si>
-    <t>Clean Up Tech</t>
-  </si>
-  <si>
-    <t>Clean Up Admin</t>
-  </si>
-  <si>
-    <t>Clean Up User</t>
-  </si>
-  <si>
-    <t>Clean Up Desk</t>
-  </si>
-  <si>
-    <t>Clean up Radio</t>
-  </si>
-  <si>
-    <t>chase</t>
-  </si>
-  <si>
     <t>Create Database Setup Instructions</t>
   </si>
   <si>
@@ -971,24 +950,6 @@
     <t>Create Diagrams</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>xxa</t>
-  </si>
-  <si>
-    <t>xxb</t>
-  </si>
-  <si>
-    <t>xxc</t>
-  </si>
-  <si>
-    <t>xxd</t>
-  </si>
-  <si>
-    <t>Create DatbaseERD</t>
-  </si>
-  <si>
     <t>Create System Models</t>
   </si>
   <si>
@@ -1013,9 +974,6 @@
     <t>Austin &amp; Cade</t>
   </si>
   <si>
-    <t>Cade &amp; Austin</t>
-  </si>
-  <si>
     <t>024</t>
   </si>
   <si>
@@ -1043,9 +1001,6 @@
     <t>Radio User Files</t>
   </si>
   <si>
-    <t>3333</t>
-  </si>
-  <si>
     <t>Create System User Manual</t>
   </si>
   <si>
@@ -1061,28 +1016,148 @@
     <t>Create Table of Contents</t>
   </si>
   <si>
-    <t>Feature 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Craete Button to open Medical Histoy </t>
-  </si>
-  <si>
-    <t>import table logic into medical history</t>
-  </si>
-  <si>
     <t>Create Table Controller</t>
   </si>
   <si>
-    <t>Fix Appearances of Mecical history page</t>
-  </si>
-  <si>
     <t>Add Table for Consent Forms in Database</t>
   </si>
   <si>
     <t>Create Add Consent Form Page</t>
   </si>
   <si>
-    <t>Inset Consent Form Page into the RIS</t>
+    <t>024b</t>
+  </si>
+  <si>
+    <t>024c</t>
+  </si>
+  <si>
+    <t>Insert Consent Form Page into the RIS</t>
+  </si>
+  <si>
+    <t>024d</t>
+  </si>
+  <si>
+    <t>Test Feature 2 Implementation</t>
+  </si>
+  <si>
+    <t>Visual Consent Form Page</t>
+  </si>
+  <si>
+    <t>New Database Table</t>
+  </si>
+  <si>
+    <t>RIS with Feature 2 Implemented</t>
+  </si>
+  <si>
+    <t>Completion of Feature 2 Implementation</t>
+  </si>
+  <si>
+    <t>Create DatabaseERD</t>
+  </si>
+  <si>
+    <t>Clean Up Tech User Files</t>
+  </si>
+  <si>
+    <t>Clean Up Doc User Files</t>
+  </si>
+  <si>
+    <t>Clean Up Admin User Files</t>
+  </si>
+  <si>
+    <t>Clean Up User User Files</t>
+  </si>
+  <si>
+    <t>Clean Up Desk User Files</t>
+  </si>
+  <si>
+    <t>Clean Up Radio User Files</t>
+  </si>
+  <si>
+    <t>025a</t>
+  </si>
+  <si>
+    <t>025b</t>
+  </si>
+  <si>
+    <t>025c</t>
+  </si>
+  <si>
+    <t>025d</t>
+  </si>
+  <si>
+    <t>025e</t>
+  </si>
+  <si>
+    <t>025f</t>
+  </si>
+  <si>
+    <t>Add Functionality to the Admin User</t>
+  </si>
+  <si>
+    <t>User Files without Errors</t>
+  </si>
+  <si>
+    <t>Doc Files without Errors</t>
+  </si>
+  <si>
+    <t>Tech Files without Errors</t>
+  </si>
+  <si>
+    <t>Admin Files without Errors</t>
+  </si>
+  <si>
+    <t>Desk Files without Errors</t>
+  </si>
+  <si>
+    <t>Radio Files without Errors</t>
+  </si>
+  <si>
+    <t>Implement Feature 3</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>Local Database</t>
+  </si>
+  <si>
+    <t>RIS System with Feature 2</t>
+  </si>
+  <si>
+    <t>Create Button to Open Medical History</t>
+  </si>
+  <si>
+    <t>Import Table Logic into Medical History</t>
+  </si>
+  <si>
+    <t>Fix Appearance of Medical History Page</t>
+  </si>
+  <si>
+    <t>026a</t>
+  </si>
+  <si>
+    <t>026b</t>
+  </si>
+  <si>
+    <t>026c</t>
+  </si>
+  <si>
+    <t>026d</t>
+  </si>
+  <si>
+    <t>026e</t>
+  </si>
+  <si>
+    <t>Implement Feature 3 into the RIS</t>
+  </si>
+  <si>
+    <t>026f</t>
+  </si>
+  <si>
+    <t>Test RIS with Feature 3 Implemented</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1710,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>699.5</c:v>
+                  <c:v>710.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3614,10 +3689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O138"/>
+  <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3690,7 +3765,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10">
         <f>SUM(E3:E100)</f>
-        <v>808</v>
+        <v>826</v>
       </c>
       <c r="F2" s="13">
         <f ca="1">TODAY() -C3</f>
@@ -3702,15 +3777,15 @@
       </c>
       <c r="H2" s="10">
         <f>SUM(H3:H100)</f>
-        <v>698.5</v>
+        <v>710.5</v>
       </c>
       <c r="I2" s="14">
         <f>SUM(I3:I100)</f>
-        <v>699.5</v>
+        <v>710.5</v>
       </c>
       <c r="J2" s="14">
         <f>SUM(J3:J100)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -3748,7 +3823,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C4" s="3">
         <v>44596</v>
@@ -3852,11 +3927,11 @@
         <v>4</v>
       </c>
       <c r="I6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>96</v>
@@ -3867,9 +3942,9 @@
       <c r="M6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="11" t="b">
+      <c r="N6" s="11" t="str">
         <f>IF(A6="","",IF(I6="","Not Started",IF(H6=I6,"Complete",IF(H6&gt;I6,"In Progress"))))</f>
-        <v>0</v>
+        <v>Complete</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -5980,6 +6055,9 @@
       <c r="A56" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="B56" s="2" t="s">
+        <v>349</v>
+      </c>
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
       <c r="E56" s="9">
@@ -6469,12 +6547,12 @@
         <v>235</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
       <c r="E68" s="9">
-        <f t="shared" ref="E68:E101" si="5">D68-C68</f>
+        <f t="shared" ref="E68:E108" si="5">D68-C68</f>
         <v>0</v>
       </c>
       <c r="F68" s="9"/>
@@ -6486,7 +6564,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="9">
-        <f t="shared" ref="J68:J101" si="6">H68-I68</f>
+        <f t="shared" ref="J68:J105" si="6">H68-I68</f>
         <v>0</v>
       </c>
       <c r="N68" s="11" t="str">
@@ -6533,7 +6611,7 @@
         <v>37</v>
       </c>
       <c r="N69" s="11" t="str">
-        <f t="shared" ref="N69:N101" si="8">IF(A69="","",IF(I69="","Not Started",IF(H69=I69,"Complete",IF(H69&gt;I69,"In Progress"))))</f>
+        <f t="shared" ref="N69:N105" si="8">IF(A69="","",IF(I69="","Not Started",IF(H69=I69,"Complete",IF(H69&gt;I69,"In Progress"))))</f>
         <v>Complete</v>
       </c>
     </row>
@@ -7504,423 +7582,902 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>296</v>
       </c>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
       <c r="E94" s="9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
+      <c r="H94" s="4">
+        <v>0</v>
+      </c>
+      <c r="I94" s="4">
+        <v>0</v>
+      </c>
       <c r="J94" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N94" s="11" t="str">
         <f t="shared" si="8"/>
-        <v>Not Started</v>
+        <v>Complete</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>345</v>
+      <c r="C95" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D95" s="22">
+        <v>44660</v>
       </c>
       <c r="E95" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
+      <c r="H95" s="4">
+        <v>0</v>
+      </c>
+      <c r="I95" s="4">
+        <v>0</v>
+      </c>
       <c r="J95" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K95" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="L95" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="M95" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="N95" s="11" t="str">
         <f t="shared" si="8"/>
-        <v>Not Started</v>
+        <v>Complete</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="B96" s="2" t="s">
-        <v>344</v>
+        <v>325</v>
+      </c>
+      <c r="C96" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D96" s="22">
+        <v>44660</v>
       </c>
       <c r="E96" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
+      <c r="H96" s="4">
+        <v>1</v>
+      </c>
+      <c r="I96" s="4">
+        <v>1</v>
+      </c>
       <c r="J96" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K96" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="L96" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="M96" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="N96" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="B97" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
+        <v>329</v>
+      </c>
+      <c r="C97" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D97" s="22">
+        <v>44660</v>
+      </c>
       <c r="E97" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
+      <c r="H97" s="4">
+        <v>5</v>
+      </c>
+      <c r="I97" s="4">
+        <v>5</v>
+      </c>
       <c r="J97" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K97" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="L97" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="M97" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="N97" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C98" s="22"/>
-      <c r="D98" s="22"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C98" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D98" s="22">
+        <v>44660</v>
+      </c>
       <c r="E98" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
+      <c r="H98" s="4">
+        <v>1</v>
+      </c>
+      <c r="I98" s="4">
+        <v>1</v>
+      </c>
       <c r="J98" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K98" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="L98" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="M98" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="N98" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C99" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D99" s="22">
+        <v>44660</v>
+      </c>
       <c r="E99" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
+      <c r="H99" s="4">
+        <v>2</v>
+      </c>
+      <c r="I99" s="4">
+        <v>2</v>
+      </c>
       <c r="J99" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K99" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="L99" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="M99" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="N99" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C100" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D100" s="22">
+        <v>44660</v>
+      </c>
       <c r="E100" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
+      <c r="H100" s="4">
+        <v>3</v>
+      </c>
+      <c r="I100" s="4">
+        <v>3</v>
+      </c>
       <c r="J100" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K100" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="L100" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="M100" s="19" t="s">
+        <v>229</v>
+      </c>
       <c r="N100" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C101" s="22"/>
-      <c r="D101" s="22"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C101" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D101" s="22">
+        <v>44660</v>
+      </c>
       <c r="E101" s="9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
+      <c r="H101" s="4">
+        <v>1</v>
+      </c>
+      <c r="I101" s="4">
+        <v>1</v>
+      </c>
       <c r="J101" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="K101" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="L101" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="M101" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="N101" s="11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C102" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D102" s="22">
+        <v>44660</v>
+      </c>
+      <c r="E102" s="9">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H102" s="4">
+        <v>1</v>
+      </c>
+      <c r="I102" s="4">
+        <v>1</v>
+      </c>
+      <c r="J102" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K102" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="L102" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="M102" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N102" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C103" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D103" s="22">
+        <v>44660</v>
+      </c>
+      <c r="E103" s="9">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H103" s="4">
+        <v>1</v>
+      </c>
+      <c r="I103" s="4">
+        <v>1</v>
+      </c>
+      <c r="J103" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K103" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="L103" s="19" t="s">
+        <v>354</v>
+      </c>
+      <c r="M103" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N103" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C104" s="22">
+        <v>44657</v>
+      </c>
+      <c r="D104" s="22">
+        <v>44660</v>
+      </c>
+      <c r="E104" s="9">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="H104" s="4">
+        <v>1</v>
+      </c>
+      <c r="I104" s="4">
+        <v>1</v>
+      </c>
+      <c r="J104" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K104" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="L104" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="M104" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="N104" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C105" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D105" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E105" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H105" s="4">
+        <v>0</v>
+      </c>
+      <c r="I105" s="4">
+        <v>0</v>
+      </c>
+      <c r="J105" s="9">
+        <v>0</v>
+      </c>
+      <c r="M105" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N105" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>Complete</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C106" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D106" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E106" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H106" s="4">
+        <v>1</v>
+      </c>
+      <c r="I106" s="4">
+        <v>1</v>
+      </c>
+      <c r="J106" s="9">
+        <v>0</v>
+      </c>
+      <c r="M106" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N106" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C107" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D107" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E107" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H107" s="4">
+        <v>6</v>
+      </c>
+      <c r="I107" s="4">
+        <v>6</v>
+      </c>
+      <c r="J107" s="9">
+        <v>0</v>
+      </c>
+      <c r="M107" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="N107" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C108" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D108" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E108" s="9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="H108" s="4">
+        <v>2</v>
+      </c>
+      <c r="I108" s="4">
+        <v>2</v>
+      </c>
+      <c r="J108" s="9">
+        <v>0</v>
+      </c>
+      <c r="M108" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N108" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C109" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D109" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E109" s="9">
+        <v>2</v>
+      </c>
+      <c r="H109" s="4">
+        <v>2</v>
+      </c>
+      <c r="I109" s="4">
+        <v>2</v>
+      </c>
+      <c r="J109" s="9">
+        <v>0</v>
+      </c>
+      <c r="M109" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="N109" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="B110" s="2" t="s">
-        <v>297</v>
+        <v>368</v>
+      </c>
+      <c r="C110" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D110" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E110" s="9">
+        <v>2</v>
       </c>
       <c r="H110" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I110" s="4">
-        <v>2</v>
-      </c>
-      <c r="K110" s="19" t="s">
-        <v>327</v>
+        <v>1</v>
+      </c>
+      <c r="J110" s="9">
+        <v>0</v>
       </c>
       <c r="M110" s="19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N110" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>369</v>
+      </c>
       <c r="B111" s="2" t="s">
-        <v>298</v>
+        <v>370</v>
+      </c>
+      <c r="C111" s="22">
+        <v>44664</v>
+      </c>
+      <c r="D111" s="22">
+        <v>44666</v>
+      </c>
+      <c r="E111" s="9">
+        <v>2</v>
       </c>
       <c r="H111" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I111" s="4">
-        <v>3</v>
-      </c>
-      <c r="K111" s="19" t="s">
-        <v>328</v>
+        <v>1</v>
+      </c>
+      <c r="J111" s="9">
+        <v>0</v>
       </c>
       <c r="M111" s="19" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="N111" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B113" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B114" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B115" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="H112" s="4">
-        <v>1</v>
-      </c>
-      <c r="I112" s="4">
-        <v>1</v>
-      </c>
-      <c r="K112" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="M112" s="19" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="H113" s="4">
-        <v>1</v>
-      </c>
-      <c r="I113" s="4">
-        <v>1</v>
-      </c>
-      <c r="K113" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="M113" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B114" s="2" t="s">
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B116" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="H114" s="4">
-        <v>1</v>
-      </c>
-      <c r="I114" s="4">
-        <v>1</v>
-      </c>
-      <c r="K114" s="19" t="s">
-        <v>331</v>
-      </c>
-      <c r="M114" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B115" s="2" t="s">
+      <c r="C116" s="22"/>
+      <c r="D116" s="22"/>
+      <c r="H116" s="4">
+        <v>0</v>
+      </c>
+      <c r="I116" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="H115" s="4">
-        <v>1</v>
-      </c>
-      <c r="I115" s="4">
-        <v>1</v>
-      </c>
-      <c r="K115" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="M115" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B116" s="2" t="s">
+      <c r="C117" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D117" s="22">
+        <v>44666</v>
+      </c>
+      <c r="H117" s="4">
+        <v>3</v>
+      </c>
+      <c r="I117" s="4">
+        <v>3</v>
+      </c>
+      <c r="M117" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C118" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D118" s="22">
+        <v>44666</v>
+      </c>
+      <c r="H118" s="4">
+        <v>3</v>
+      </c>
+      <c r="I118" s="4">
+        <v>3</v>
+      </c>
+      <c r="M118" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B119" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="M116" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="M117" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B118" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="M118" s="19" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>308</v>
+      <c r="C119" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D119" s="22">
+        <v>44666</v>
+      </c>
+      <c r="H119" s="4">
+        <v>3</v>
+      </c>
+      <c r="I119" s="4">
+        <v>3</v>
+      </c>
+      <c r="J119" s="9">
+        <v>0</v>
       </c>
       <c r="M119" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>310</v>
-      </c>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
+      </c>
+      <c r="C120" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D120" s="22">
+        <v>44666</v>
+      </c>
+      <c r="H120" s="4">
+        <v>3</v>
+      </c>
+      <c r="I120" s="4">
+        <v>3</v>
+      </c>
+      <c r="J120" s="9">
+        <v>0</v>
       </c>
       <c r="M120" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>311</v>
-      </c>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>315</v>
+        <v>305</v>
+      </c>
+      <c r="C121" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D121" s="22">
+        <v>44665</v>
+      </c>
+      <c r="H121" s="4">
+        <v>1</v>
+      </c>
+      <c r="I121" s="4">
+        <v>1</v>
+      </c>
+      <c r="J121" s="9">
+        <v>0</v>
       </c>
       <c r="M121" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>312</v>
-      </c>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
+      </c>
+      <c r="C122" s="22">
+        <v>44665</v>
+      </c>
+      <c r="D122" s="22">
+        <v>44665</v>
+      </c>
+      <c r="H122" s="4">
+        <v>3</v>
+      </c>
+      <c r="I122" s="4">
+        <v>3</v>
+      </c>
+      <c r="J122" s="9">
+        <v>0</v>
       </c>
       <c r="M122" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="M123" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B124" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="M124" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B125" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="M125" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C124" s="22"/>
+      <c r="D124" s="22"/>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C125" s="22"/>
+      <c r="D125" s="22"/>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="M126" s="19" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="M127" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
     <row r="129" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>335</v>
+        <v>320</v>
+      </c>
+      <c r="M129" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="M130" s="19" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="131" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="134" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B134" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="135" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B135" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="136" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B136" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="137" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B137" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="138" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B138" s="2" t="s">
-        <v>343</v>
+        <v>323</v>
+      </c>
+      <c r="M131" s="19" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>